<commit_message>
Updated for provisional acceptance.
</commit_message>
<xml_diff>
--- a/public_use_dataset.xlsx
+++ b/public_use_dataset.xlsx
@@ -8,13 +8,12 @@
   <sheets>
     <sheet name="Studies" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Findings" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Notes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="857">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -2605,9 +2604,6 @@
   </si>
   <si>
     <t xml:space="preserve">GRADE-Word Meaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These data are made available under an Attribution-Non-Commercial 4.0 Creative Commons License. You may use, share, and adapt the data so long as you agree to acknowledge this project as the source of these data. Please cite the data as: Neitzel, A.J., Lake, C., Pellegrini, M., &amp; Slavin, R.E. (2020). Data archive for "A Synthesis of Quantitative Research on Programs For Struggling Readers in Elementary Schools." Towson, MD: Center for Research and Reform in Education (CRRE), Johns Hopkins University. Retrieved from https://github.com/aj-neitzel/A-Synthesis-of-Quantitative-Research-on-Programs-For-Struggling-Readers-in-Elementary-Schools</t>
   </si>
 </sst>
 </file>
@@ -18316,23 +18312,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>